<commit_message>
Added new statements, not tested
</commit_message>
<xml_diff>
--- a/Documentation/CSharpSyntaxKindList.xlsx
+++ b/Documentation/CSharpSyntaxKindList.xlsx
@@ -2305,8 +2305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D512"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A483" workbookViewId="0">
-      <selection activeCell="D512" sqref="D512"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="B298" sqref="B298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4743,6 +4743,9 @@
       <c r="B293" s="4" t="s">
         <v>279</v>
       </c>
+      <c r="C293">
+        <v>1</v>
+      </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
@@ -6942,7 +6945,7 @@
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C512">
         <f>SUM(C1:C511)</f>
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D512">
         <f>SUM(D1:D511)</f>

</xml_diff>

<commit_message>
Shelved in middle of whitespace nightmare
</commit_message>
<xml_diff>
--- a/Documentation/CSharpSyntaxKindList.xlsx
+++ b/Documentation/CSharpSyntaxKindList.xlsx
@@ -2305,8 +2305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D512"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
-      <selection activeCell="B298" sqref="B298"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="C239" sqref="C239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3980,7 +3980,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>214</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>215</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>216</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>217</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>218</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>219</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>220</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>221</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>222</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>223</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>224</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>225</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>226</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>227</v>
       </c>
@@ -4092,20 +4092,26 @@
         <v>212</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>228</v>
       </c>
       <c r="B223" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>229</v>
       </c>
       <c r="B224" s="4" t="s">
         <v>214</v>
+      </c>
+      <c r="C224">
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -4263,6 +4269,9 @@
       <c r="B239" s="4" t="s">
         <v>229</v>
       </c>
+      <c r="C239">
+        <v>1</v>
+      </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
@@ -6945,7 +6954,7 @@
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C512">
         <f>SUM(C1:C511)</f>
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D512">
         <f>SUM(D1:D511)</f>

</xml_diff>